<commit_message>
encryption implementation and telegram user problem fixed
</commit_message>
<xml_diff>
--- a/bridge/database/export/punti_raccolta.xlsx
+++ b/bridge/database/export/punti_raccolta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -32,6 +32,15 @@
   </si>
   <si>
     <t>test_acquisition_point</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -363,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -391,6 +400,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>